<commit_message>
update XL til 2016-04-02
</commit_message>
<xml_diff>
--- a/Tageslänge.xlsx
+++ b/Tageslänge.xlsx
@@ -560,6 +560,150 @@
                 <c:pt idx="99">
                   <c:v>42458</c:v>
                 </c:pt>
+                <c:pt idx="100">
+                  <c:v>42459</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>42460</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>42461</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>42462</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>42463</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>42464</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>42465</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>42466</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>42467</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>42468</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>42469</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>42470</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>42471</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>42472</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>42473</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>42474</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>42475</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>42476</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>42477</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>42478</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>42479</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>42480</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>42481</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>42482</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>42483</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>42484</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>42485</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>42486</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>42487</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>42488</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>42489</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>42490</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>42491</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>42492</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>42493</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>42494</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>42495</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>42496</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>42497</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>42498</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>42499</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>42500</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>42501</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>42502</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>42503</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>42504</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>42505</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>42506</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -849,24 +993,168 @@
                   <c:v>0.51249999999999996</c:v>
                 </c:pt>
                 <c:pt idx="93">
+                  <c:v>0.51458333333333317</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.51736111111111116</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.51944444444444449</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.52222222222222225</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.52430555555555558</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.52708333333333335</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.52916666666666679</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.53194444444444433</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.53402777777777777</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.53680555555555565</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.5395833333333333</c:v>
+                </c:pt>
+                <c:pt idx="104">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="94">
+                <c:pt idx="105">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="95">
+                <c:pt idx="106">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="96">
+                <c:pt idx="107">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="97">
+                <c:pt idx="108">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="98">
+                <c:pt idx="109">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="99">
+                <c:pt idx="110">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="147">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -884,11 +1172,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="98413952"/>
-        <c:axId val="98415744"/>
+        <c:axId val="88190336"/>
+        <c:axId val="88196224"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="98413952"/>
+        <c:axId val="88190336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -898,14 +1186,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98415744"/>
+        <c:crossAx val="88196224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="98415744"/>
+        <c:axId val="88196224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -916,7 +1204,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="98413952"/>
+        <c:crossAx val="88190336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1255,12 +1543,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E102"/>
+  <dimension ref="A1:E258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1500" topLeftCell="A40" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1500" topLeftCell="A48" activePane="bottomLeft"/>
       <selection activeCell="E1" activeCellId="1" sqref="B1:B1048576 E1:E1048576"/>
-      <selection pane="bottomLeft" activeCell="C96" sqref="C96"/>
+      <selection pane="bottomLeft" activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2928,9 +3216,15 @@
       <c r="B96" s="5">
         <v>42452</v>
       </c>
+      <c r="C96" s="2">
+        <v>0.25694444444444448</v>
+      </c>
+      <c r="D96" s="2">
+        <v>0.7715277777777777</v>
+      </c>
       <c r="E96" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.51458333333333317</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2941,9 +3235,15 @@
       <c r="B97" s="5">
         <v>42453</v>
       </c>
+      <c r="C97" s="2">
+        <v>0.25555555555555559</v>
+      </c>
+      <c r="D97" s="2">
+        <v>0.7729166666666667</v>
+      </c>
       <c r="E97" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.51736111111111116</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2954,9 +3254,15 @@
       <c r="B98" s="5">
         <v>42454</v>
       </c>
+      <c r="C98" s="2">
+        <v>0.25416666666666665</v>
+      </c>
+      <c r="D98" s="2">
+        <v>0.77361111111111114</v>
+      </c>
       <c r="E98" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.51944444444444449</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2967,9 +3273,15 @@
       <c r="B99" s="5">
         <v>42455</v>
       </c>
+      <c r="C99" s="2">
+        <v>0.25277777777777777</v>
+      </c>
+      <c r="D99" s="2">
+        <v>0.77500000000000002</v>
+      </c>
       <c r="E99" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.52222222222222225</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2980,9 +3292,15 @@
       <c r="B100" s="5">
         <v>42456</v>
       </c>
+      <c r="C100" s="2">
+        <v>0.29305555555555557</v>
+      </c>
+      <c r="D100" s="2">
+        <v>0.81736111111111109</v>
+      </c>
       <c r="E100" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.52430555555555558</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2993,9 +3311,15 @@
       <c r="B101" s="5">
         <v>42457</v>
       </c>
+      <c r="C101" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="D101" s="2">
+        <v>0.81874999999999998</v>
+      </c>
       <c r="E101" s="2">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>0.52708333333333335</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -3006,8 +3330,2066 @@
       <c r="B102" s="5">
         <v>42458</v>
       </c>
+      <c r="C102" s="2">
+        <v>0.2902777777777778</v>
+      </c>
+      <c r="D102" s="2">
+        <v>0.81944444444444453</v>
+      </c>
       <c r="E102" s="2">
         <f t="shared" si="5"/>
+        <v>0.52916666666666679</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="4">
+        <f t="shared" ref="A103:A166" si="6">B103</f>
+        <v>42459</v>
+      </c>
+      <c r="B103" s="5">
+        <v>42459</v>
+      </c>
+      <c r="C103" s="2">
+        <v>0.28888888888888892</v>
+      </c>
+      <c r="D103" s="2">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="E103" s="2">
+        <f t="shared" ref="E103:E166" si="7">D103-C103</f>
+        <v>0.53194444444444433</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="4">
+        <f t="shared" si="6"/>
+        <v>42460</v>
+      </c>
+      <c r="B104" s="5">
+        <v>42460</v>
+      </c>
+      <c r="C104" s="2">
+        <v>0.28750000000000003</v>
+      </c>
+      <c r="D104" s="2">
+        <v>0.82152777777777775</v>
+      </c>
+      <c r="E104" s="2">
+        <f t="shared" si="7"/>
+        <v>0.53402777777777777</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="4">
+        <f t="shared" si="6"/>
+        <v>42461</v>
+      </c>
+      <c r="B105" s="5">
+        <v>42461</v>
+      </c>
+      <c r="C105" s="2">
+        <v>0.28541666666666665</v>
+      </c>
+      <c r="D105" s="2">
+        <v>0.8222222222222223</v>
+      </c>
+      <c r="E105" s="2">
+        <f t="shared" si="7"/>
+        <v>0.53680555555555565</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="4">
+        <f t="shared" si="6"/>
+        <v>42462</v>
+      </c>
+      <c r="B106" s="5">
+        <v>42462</v>
+      </c>
+      <c r="C106" s="2">
+        <v>0.28402777777777777</v>
+      </c>
+      <c r="D106" s="2">
+        <v>0.82361111111111107</v>
+      </c>
+      <c r="E106" s="2">
+        <f t="shared" si="7"/>
+        <v>0.5395833333333333</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="4">
+        <f t="shared" si="6"/>
+        <v>42463</v>
+      </c>
+      <c r="B107" s="5">
+        <v>42463</v>
+      </c>
+      <c r="E107" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="4">
+        <f t="shared" si="6"/>
+        <v>42464</v>
+      </c>
+      <c r="B108" s="5">
+        <v>42464</v>
+      </c>
+      <c r="E108" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="4">
+        <f t="shared" si="6"/>
+        <v>42465</v>
+      </c>
+      <c r="B109" s="5">
+        <v>42465</v>
+      </c>
+      <c r="E109" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="4">
+        <f t="shared" si="6"/>
+        <v>42466</v>
+      </c>
+      <c r="B110" s="5">
+        <v>42466</v>
+      </c>
+      <c r="E110" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="4">
+        <f t="shared" si="6"/>
+        <v>42467</v>
+      </c>
+      <c r="B111" s="5">
+        <v>42467</v>
+      </c>
+      <c r="E111" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="4">
+        <f t="shared" si="6"/>
+        <v>42468</v>
+      </c>
+      <c r="B112" s="5">
+        <v>42468</v>
+      </c>
+      <c r="E112" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="4">
+        <f t="shared" si="6"/>
+        <v>42469</v>
+      </c>
+      <c r="B113" s="5">
+        <v>42469</v>
+      </c>
+      <c r="E113" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="4">
+        <f t="shared" si="6"/>
+        <v>42470</v>
+      </c>
+      <c r="B114" s="5">
+        <v>42470</v>
+      </c>
+      <c r="E114" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="4">
+        <f t="shared" si="6"/>
+        <v>42471</v>
+      </c>
+      <c r="B115" s="5">
+        <v>42471</v>
+      </c>
+      <c r="E115" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="4">
+        <f t="shared" si="6"/>
+        <v>42472</v>
+      </c>
+      <c r="B116" s="5">
+        <v>42472</v>
+      </c>
+      <c r="E116" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="4">
+        <f t="shared" si="6"/>
+        <v>42473</v>
+      </c>
+      <c r="B117" s="5">
+        <v>42473</v>
+      </c>
+      <c r="E117" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="4">
+        <f t="shared" si="6"/>
+        <v>42474</v>
+      </c>
+      <c r="B118" s="5">
+        <v>42474</v>
+      </c>
+      <c r="E118" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="4">
+        <f t="shared" si="6"/>
+        <v>42475</v>
+      </c>
+      <c r="B119" s="5">
+        <v>42475</v>
+      </c>
+      <c r="E119" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="4">
+        <f t="shared" si="6"/>
+        <v>42476</v>
+      </c>
+      <c r="B120" s="5">
+        <v>42476</v>
+      </c>
+      <c r="E120" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="4">
+        <f t="shared" si="6"/>
+        <v>42477</v>
+      </c>
+      <c r="B121" s="5">
+        <v>42477</v>
+      </c>
+      <c r="E121" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="4">
+        <f t="shared" si="6"/>
+        <v>42478</v>
+      </c>
+      <c r="B122" s="5">
+        <v>42478</v>
+      </c>
+      <c r="E122" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="4">
+        <f t="shared" si="6"/>
+        <v>42479</v>
+      </c>
+      <c r="B123" s="5">
+        <v>42479</v>
+      </c>
+      <c r="E123" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="4">
+        <f t="shared" si="6"/>
+        <v>42480</v>
+      </c>
+      <c r="B124" s="5">
+        <v>42480</v>
+      </c>
+      <c r="E124" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="4">
+        <f t="shared" si="6"/>
+        <v>42481</v>
+      </c>
+      <c r="B125" s="5">
+        <v>42481</v>
+      </c>
+      <c r="E125" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="4">
+        <f t="shared" si="6"/>
+        <v>42482</v>
+      </c>
+      <c r="B126" s="5">
+        <v>42482</v>
+      </c>
+      <c r="E126" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="4">
+        <f t="shared" si="6"/>
+        <v>42483</v>
+      </c>
+      <c r="B127" s="5">
+        <v>42483</v>
+      </c>
+      <c r="E127" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="4">
+        <f t="shared" si="6"/>
+        <v>42484</v>
+      </c>
+      <c r="B128" s="5">
+        <v>42484</v>
+      </c>
+      <c r="E128" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="4">
+        <f t="shared" si="6"/>
+        <v>42485</v>
+      </c>
+      <c r="B129" s="5">
+        <v>42485</v>
+      </c>
+      <c r="E129" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="4">
+        <f t="shared" si="6"/>
+        <v>42486</v>
+      </c>
+      <c r="B130" s="5">
+        <v>42486</v>
+      </c>
+      <c r="E130" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="4">
+        <f t="shared" si="6"/>
+        <v>42487</v>
+      </c>
+      <c r="B131" s="5">
+        <v>42487</v>
+      </c>
+      <c r="E131" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="4">
+        <f t="shared" si="6"/>
+        <v>42488</v>
+      </c>
+      <c r="B132" s="5">
+        <v>42488</v>
+      </c>
+      <c r="E132" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="4">
+        <f t="shared" si="6"/>
+        <v>42489</v>
+      </c>
+      <c r="B133" s="5">
+        <v>42489</v>
+      </c>
+      <c r="E133" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="4">
+        <f t="shared" si="6"/>
+        <v>42490</v>
+      </c>
+      <c r="B134" s="5">
+        <v>42490</v>
+      </c>
+      <c r="E134" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="4">
+        <f t="shared" si="6"/>
+        <v>42491</v>
+      </c>
+      <c r="B135" s="5">
+        <v>42491</v>
+      </c>
+      <c r="E135" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="4">
+        <f t="shared" si="6"/>
+        <v>42492</v>
+      </c>
+      <c r="B136" s="5">
+        <v>42492</v>
+      </c>
+      <c r="E136" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="4">
+        <f t="shared" si="6"/>
+        <v>42493</v>
+      </c>
+      <c r="B137" s="5">
+        <v>42493</v>
+      </c>
+      <c r="E137" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="4">
+        <f t="shared" si="6"/>
+        <v>42494</v>
+      </c>
+      <c r="B138" s="5">
+        <v>42494</v>
+      </c>
+      <c r="E138" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="4">
+        <f t="shared" si="6"/>
+        <v>42495</v>
+      </c>
+      <c r="B139" s="5">
+        <v>42495</v>
+      </c>
+      <c r="E139" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="4">
+        <f t="shared" si="6"/>
+        <v>42496</v>
+      </c>
+      <c r="B140" s="5">
+        <v>42496</v>
+      </c>
+      <c r="E140" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="4">
+        <f t="shared" si="6"/>
+        <v>42497</v>
+      </c>
+      <c r="B141" s="5">
+        <v>42497</v>
+      </c>
+      <c r="E141" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="4">
+        <f t="shared" si="6"/>
+        <v>42498</v>
+      </c>
+      <c r="B142" s="5">
+        <v>42498</v>
+      </c>
+      <c r="E142" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="4">
+        <f t="shared" si="6"/>
+        <v>42499</v>
+      </c>
+      <c r="B143" s="5">
+        <v>42499</v>
+      </c>
+      <c r="E143" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="4">
+        <f t="shared" si="6"/>
+        <v>42500</v>
+      </c>
+      <c r="B144" s="5">
+        <v>42500</v>
+      </c>
+      <c r="E144" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" s="4">
+        <f t="shared" si="6"/>
+        <v>42501</v>
+      </c>
+      <c r="B145" s="5">
+        <v>42501</v>
+      </c>
+      <c r="E145" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="4">
+        <f t="shared" si="6"/>
+        <v>42502</v>
+      </c>
+      <c r="B146" s="5">
+        <v>42502</v>
+      </c>
+      <c r="E146" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="4">
+        <f t="shared" si="6"/>
+        <v>42503</v>
+      </c>
+      <c r="B147" s="5">
+        <v>42503</v>
+      </c>
+      <c r="E147" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="4">
+        <f t="shared" si="6"/>
+        <v>42504</v>
+      </c>
+      <c r="B148" s="5">
+        <v>42504</v>
+      </c>
+      <c r="E148" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" s="4">
+        <f t="shared" si="6"/>
+        <v>42505</v>
+      </c>
+      <c r="B149" s="5">
+        <v>42505</v>
+      </c>
+      <c r="E149" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" s="4">
+        <f t="shared" si="6"/>
+        <v>42506</v>
+      </c>
+      <c r="B150" s="5">
+        <v>42506</v>
+      </c>
+      <c r="E150" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" s="4">
+        <f t="shared" si="6"/>
+        <v>42507</v>
+      </c>
+      <c r="B151" s="5">
+        <v>42507</v>
+      </c>
+      <c r="E151" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" s="4">
+        <f t="shared" si="6"/>
+        <v>42508</v>
+      </c>
+      <c r="B152" s="5">
+        <v>42508</v>
+      </c>
+      <c r="E152" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" s="4">
+        <f t="shared" si="6"/>
+        <v>42509</v>
+      </c>
+      <c r="B153" s="5">
+        <v>42509</v>
+      </c>
+      <c r="E153" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" s="4">
+        <f t="shared" si="6"/>
+        <v>42510</v>
+      </c>
+      <c r="B154" s="5">
+        <v>42510</v>
+      </c>
+      <c r="E154" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" s="4">
+        <f t="shared" si="6"/>
+        <v>42511</v>
+      </c>
+      <c r="B155" s="5">
+        <v>42511</v>
+      </c>
+      <c r="E155" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" s="4">
+        <f t="shared" si="6"/>
+        <v>42512</v>
+      </c>
+      <c r="B156" s="5">
+        <v>42512</v>
+      </c>
+      <c r="E156" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" s="4">
+        <f t="shared" si="6"/>
+        <v>42513</v>
+      </c>
+      <c r="B157" s="5">
+        <v>42513</v>
+      </c>
+      <c r="E157" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" s="4">
+        <f t="shared" si="6"/>
+        <v>42514</v>
+      </c>
+      <c r="B158" s="5">
+        <v>42514</v>
+      </c>
+      <c r="E158" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="4">
+        <f t="shared" si="6"/>
+        <v>42515</v>
+      </c>
+      <c r="B159" s="5">
+        <v>42515</v>
+      </c>
+      <c r="E159" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="4">
+        <f t="shared" si="6"/>
+        <v>42516</v>
+      </c>
+      <c r="B160" s="5">
+        <v>42516</v>
+      </c>
+      <c r="E160" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="4">
+        <f t="shared" si="6"/>
+        <v>42517</v>
+      </c>
+      <c r="B161" s="5">
+        <v>42517</v>
+      </c>
+      <c r="E161" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" s="4">
+        <f t="shared" si="6"/>
+        <v>42518</v>
+      </c>
+      <c r="B162" s="5">
+        <v>42518</v>
+      </c>
+      <c r="E162" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" s="4">
+        <f t="shared" si="6"/>
+        <v>42519</v>
+      </c>
+      <c r="B163" s="5">
+        <v>42519</v>
+      </c>
+      <c r="E163" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" s="4">
+        <f t="shared" si="6"/>
+        <v>42520</v>
+      </c>
+      <c r="B164" s="5">
+        <v>42520</v>
+      </c>
+      <c r="E164" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" s="4">
+        <f t="shared" si="6"/>
+        <v>42521</v>
+      </c>
+      <c r="B165" s="5">
+        <v>42521</v>
+      </c>
+      <c r="E165" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" s="4">
+        <f t="shared" si="6"/>
+        <v>42522</v>
+      </c>
+      <c r="B166" s="5">
+        <v>42522</v>
+      </c>
+      <c r="E166" s="2">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" s="4">
+        <f t="shared" ref="A167:A230" si="8">B167</f>
+        <v>42523</v>
+      </c>
+      <c r="B167" s="5">
+        <v>42523</v>
+      </c>
+      <c r="E167" s="2">
+        <f t="shared" ref="E167:E230" si="9">D167-C167</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" s="4">
+        <f t="shared" si="8"/>
+        <v>42524</v>
+      </c>
+      <c r="B168" s="5">
+        <v>42524</v>
+      </c>
+      <c r="E168" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" s="4">
+        <f t="shared" si="8"/>
+        <v>42525</v>
+      </c>
+      <c r="B169" s="5">
+        <v>42525</v>
+      </c>
+      <c r="E169" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="4">
+        <f t="shared" si="8"/>
+        <v>42526</v>
+      </c>
+      <c r="B170" s="5">
+        <v>42526</v>
+      </c>
+      <c r="E170" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="4">
+        <f t="shared" si="8"/>
+        <v>42527</v>
+      </c>
+      <c r="B171" s="5">
+        <v>42527</v>
+      </c>
+      <c r="E171" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="4">
+        <f t="shared" si="8"/>
+        <v>42528</v>
+      </c>
+      <c r="B172" s="5">
+        <v>42528</v>
+      </c>
+      <c r="E172" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="4">
+        <f t="shared" si="8"/>
+        <v>42529</v>
+      </c>
+      <c r="B173" s="5">
+        <v>42529</v>
+      </c>
+      <c r="E173" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="4">
+        <f t="shared" si="8"/>
+        <v>42530</v>
+      </c>
+      <c r="B174" s="5">
+        <v>42530</v>
+      </c>
+      <c r="E174" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="4">
+        <f t="shared" si="8"/>
+        <v>42531</v>
+      </c>
+      <c r="B175" s="5">
+        <v>42531</v>
+      </c>
+      <c r="E175" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="4">
+        <f t="shared" si="8"/>
+        <v>42532</v>
+      </c>
+      <c r="B176" s="5">
+        <v>42532</v>
+      </c>
+      <c r="E176" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="4">
+        <f t="shared" si="8"/>
+        <v>42533</v>
+      </c>
+      <c r="B177" s="5">
+        <v>42533</v>
+      </c>
+      <c r="E177" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="4">
+        <f t="shared" si="8"/>
+        <v>42534</v>
+      </c>
+      <c r="B178" s="5">
+        <v>42534</v>
+      </c>
+      <c r="E178" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="4">
+        <f t="shared" si="8"/>
+        <v>42535</v>
+      </c>
+      <c r="B179" s="5">
+        <v>42535</v>
+      </c>
+      <c r="E179" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="4">
+        <f t="shared" si="8"/>
+        <v>42536</v>
+      </c>
+      <c r="B180" s="5">
+        <v>42536</v>
+      </c>
+      <c r="E180" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="4">
+        <f t="shared" si="8"/>
+        <v>42537</v>
+      </c>
+      <c r="B181" s="5">
+        <v>42537</v>
+      </c>
+      <c r="E181" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="4">
+        <f t="shared" si="8"/>
+        <v>42538</v>
+      </c>
+      <c r="B182" s="5">
+        <v>42538</v>
+      </c>
+      <c r="E182" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="4">
+        <f t="shared" si="8"/>
+        <v>42539</v>
+      </c>
+      <c r="B183" s="5">
+        <v>42539</v>
+      </c>
+      <c r="E183" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="4">
+        <f t="shared" si="8"/>
+        <v>42540</v>
+      </c>
+      <c r="B184" s="5">
+        <v>42540</v>
+      </c>
+      <c r="E184" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="4">
+        <f t="shared" si="8"/>
+        <v>42541</v>
+      </c>
+      <c r="B185" s="5">
+        <v>42541</v>
+      </c>
+      <c r="E185" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="4">
+        <f t="shared" si="8"/>
+        <v>42542</v>
+      </c>
+      <c r="B186" s="5">
+        <v>42542</v>
+      </c>
+      <c r="E186" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="4">
+        <f t="shared" si="8"/>
+        <v>42543</v>
+      </c>
+      <c r="B187" s="5">
+        <v>42543</v>
+      </c>
+      <c r="E187" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="4">
+        <f t="shared" si="8"/>
+        <v>42544</v>
+      </c>
+      <c r="B188" s="5">
+        <v>42544</v>
+      </c>
+      <c r="E188" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="4">
+        <f t="shared" si="8"/>
+        <v>42545</v>
+      </c>
+      <c r="B189" s="5">
+        <v>42545</v>
+      </c>
+      <c r="E189" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="4">
+        <f t="shared" si="8"/>
+        <v>42546</v>
+      </c>
+      <c r="B190" s="5">
+        <v>42546</v>
+      </c>
+      <c r="E190" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="4">
+        <f t="shared" si="8"/>
+        <v>42547</v>
+      </c>
+      <c r="B191" s="5">
+        <v>42547</v>
+      </c>
+      <c r="E191" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="4">
+        <f t="shared" si="8"/>
+        <v>42548</v>
+      </c>
+      <c r="B192" s="5">
+        <v>42548</v>
+      </c>
+      <c r="E192" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="4">
+        <f t="shared" si="8"/>
+        <v>42549</v>
+      </c>
+      <c r="B193" s="5">
+        <v>42549</v>
+      </c>
+      <c r="E193" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="4">
+        <f t="shared" si="8"/>
+        <v>42550</v>
+      </c>
+      <c r="B194" s="5">
+        <v>42550</v>
+      </c>
+      <c r="E194" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="4">
+        <f t="shared" si="8"/>
+        <v>42551</v>
+      </c>
+      <c r="B195" s="5">
+        <v>42551</v>
+      </c>
+      <c r="E195" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="4">
+        <f t="shared" si="8"/>
+        <v>42552</v>
+      </c>
+      <c r="B196" s="5">
+        <v>42552</v>
+      </c>
+      <c r="E196" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="4">
+        <f t="shared" si="8"/>
+        <v>42553</v>
+      </c>
+      <c r="B197" s="5">
+        <v>42553</v>
+      </c>
+      <c r="E197" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="4">
+        <f t="shared" si="8"/>
+        <v>42554</v>
+      </c>
+      <c r="B198" s="5">
+        <v>42554</v>
+      </c>
+      <c r="E198" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="4">
+        <f t="shared" si="8"/>
+        <v>42555</v>
+      </c>
+      <c r="B199" s="5">
+        <v>42555</v>
+      </c>
+      <c r="E199" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="4">
+        <f t="shared" si="8"/>
+        <v>42556</v>
+      </c>
+      <c r="B200" s="5">
+        <v>42556</v>
+      </c>
+      <c r="E200" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="4">
+        <f t="shared" si="8"/>
+        <v>42557</v>
+      </c>
+      <c r="B201" s="5">
+        <v>42557</v>
+      </c>
+      <c r="E201" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="4">
+        <f t="shared" si="8"/>
+        <v>42558</v>
+      </c>
+      <c r="B202" s="5">
+        <v>42558</v>
+      </c>
+      <c r="E202" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="4">
+        <f t="shared" si="8"/>
+        <v>42559</v>
+      </c>
+      <c r="B203" s="5">
+        <v>42559</v>
+      </c>
+      <c r="E203" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="4">
+        <f t="shared" si="8"/>
+        <v>42560</v>
+      </c>
+      <c r="B204" s="5">
+        <v>42560</v>
+      </c>
+      <c r="E204" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="4">
+        <f t="shared" si="8"/>
+        <v>42561</v>
+      </c>
+      <c r="B205" s="5">
+        <v>42561</v>
+      </c>
+      <c r="E205" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="4">
+        <f t="shared" si="8"/>
+        <v>42562</v>
+      </c>
+      <c r="B206" s="5">
+        <v>42562</v>
+      </c>
+      <c r="E206" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="4">
+        <f t="shared" si="8"/>
+        <v>42563</v>
+      </c>
+      <c r="B207" s="5">
+        <v>42563</v>
+      </c>
+      <c r="E207" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="4">
+        <f t="shared" si="8"/>
+        <v>42564</v>
+      </c>
+      <c r="B208" s="5">
+        <v>42564</v>
+      </c>
+      <c r="E208" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A209" s="4">
+        <f t="shared" si="8"/>
+        <v>42565</v>
+      </c>
+      <c r="B209" s="5">
+        <v>42565</v>
+      </c>
+      <c r="E209" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="4">
+        <f t="shared" si="8"/>
+        <v>42566</v>
+      </c>
+      <c r="B210" s="5">
+        <v>42566</v>
+      </c>
+      <c r="E210" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="4">
+        <f t="shared" si="8"/>
+        <v>42567</v>
+      </c>
+      <c r="B211" s="5">
+        <v>42567</v>
+      </c>
+      <c r="E211" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A212" s="4">
+        <f t="shared" si="8"/>
+        <v>42568</v>
+      </c>
+      <c r="B212" s="5">
+        <v>42568</v>
+      </c>
+      <c r="E212" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="4">
+        <f t="shared" si="8"/>
+        <v>42569</v>
+      </c>
+      <c r="B213" s="5">
+        <v>42569</v>
+      </c>
+      <c r="E213" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="4">
+        <f t="shared" si="8"/>
+        <v>42570</v>
+      </c>
+      <c r="B214" s="5">
+        <v>42570</v>
+      </c>
+      <c r="E214" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="4">
+        <f t="shared" si="8"/>
+        <v>42571</v>
+      </c>
+      <c r="B215" s="5">
+        <v>42571</v>
+      </c>
+      <c r="E215" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="4">
+        <f t="shared" si="8"/>
+        <v>42572</v>
+      </c>
+      <c r="B216" s="5">
+        <v>42572</v>
+      </c>
+      <c r="E216" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="4">
+        <f t="shared" si="8"/>
+        <v>42573</v>
+      </c>
+      <c r="B217" s="5">
+        <v>42573</v>
+      </c>
+      <c r="E217" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="4">
+        <f t="shared" si="8"/>
+        <v>42574</v>
+      </c>
+      <c r="B218" s="5">
+        <v>42574</v>
+      </c>
+      <c r="E218" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="4">
+        <f t="shared" si="8"/>
+        <v>42575</v>
+      </c>
+      <c r="B219" s="5">
+        <v>42575</v>
+      </c>
+      <c r="E219" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="4">
+        <f t="shared" si="8"/>
+        <v>42576</v>
+      </c>
+      <c r="B220" s="5">
+        <v>42576</v>
+      </c>
+      <c r="E220" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="4">
+        <f t="shared" si="8"/>
+        <v>42577</v>
+      </c>
+      <c r="B221" s="5">
+        <v>42577</v>
+      </c>
+      <c r="E221" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="4">
+        <f t="shared" si="8"/>
+        <v>42578</v>
+      </c>
+      <c r="B222" s="5">
+        <v>42578</v>
+      </c>
+      <c r="E222" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="4">
+        <f t="shared" si="8"/>
+        <v>42579</v>
+      </c>
+      <c r="B223" s="5">
+        <v>42579</v>
+      </c>
+      <c r="E223" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="4">
+        <f t="shared" si="8"/>
+        <v>42580</v>
+      </c>
+      <c r="B224" s="5">
+        <v>42580</v>
+      </c>
+      <c r="E224" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="4">
+        <f t="shared" si="8"/>
+        <v>42581</v>
+      </c>
+      <c r="B225" s="5">
+        <v>42581</v>
+      </c>
+      <c r="E225" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A226" s="4">
+        <f t="shared" si="8"/>
+        <v>42582</v>
+      </c>
+      <c r="B226" s="5">
+        <v>42582</v>
+      </c>
+      <c r="E226" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A227" s="4">
+        <f t="shared" si="8"/>
+        <v>42583</v>
+      </c>
+      <c r="B227" s="5">
+        <v>42583</v>
+      </c>
+      <c r="E227" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="4">
+        <f t="shared" si="8"/>
+        <v>42584</v>
+      </c>
+      <c r="B228" s="5">
+        <v>42584</v>
+      </c>
+      <c r="E228" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="4">
+        <f t="shared" si="8"/>
+        <v>42585</v>
+      </c>
+      <c r="B229" s="5">
+        <v>42585</v>
+      </c>
+      <c r="E229" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="4">
+        <f t="shared" si="8"/>
+        <v>42586</v>
+      </c>
+      <c r="B230" s="5">
+        <v>42586</v>
+      </c>
+      <c r="E230" s="2">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A231" s="4">
+        <f t="shared" ref="A231:A258" si="10">B231</f>
+        <v>42587</v>
+      </c>
+      <c r="B231" s="5">
+        <v>42587</v>
+      </c>
+      <c r="E231" s="2">
+        <f t="shared" ref="E231:E258" si="11">D231-C231</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="4">
+        <f t="shared" si="10"/>
+        <v>42588</v>
+      </c>
+      <c r="B232" s="5">
+        <v>42588</v>
+      </c>
+      <c r="E232" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A233" s="4">
+        <f t="shared" si="10"/>
+        <v>42589</v>
+      </c>
+      <c r="B233" s="5">
+        <v>42589</v>
+      </c>
+      <c r="E233" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A234" s="4">
+        <f t="shared" si="10"/>
+        <v>42590</v>
+      </c>
+      <c r="B234" s="5">
+        <v>42590</v>
+      </c>
+      <c r="E234" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A235" s="4">
+        <f t="shared" si="10"/>
+        <v>42591</v>
+      </c>
+      <c r="B235" s="5">
+        <v>42591</v>
+      </c>
+      <c r="E235" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A236" s="4">
+        <f t="shared" si="10"/>
+        <v>42592</v>
+      </c>
+      <c r="B236" s="5">
+        <v>42592</v>
+      </c>
+      <c r="E236" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A237" s="4">
+        <f t="shared" si="10"/>
+        <v>42593</v>
+      </c>
+      <c r="B237" s="5">
+        <v>42593</v>
+      </c>
+      <c r="E237" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A238" s="4">
+        <f t="shared" si="10"/>
+        <v>42594</v>
+      </c>
+      <c r="B238" s="5">
+        <v>42594</v>
+      </c>
+      <c r="E238" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" s="4">
+        <f t="shared" si="10"/>
+        <v>42595</v>
+      </c>
+      <c r="B239" s="5">
+        <v>42595</v>
+      </c>
+      <c r="E239" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" s="4">
+        <f t="shared" si="10"/>
+        <v>42596</v>
+      </c>
+      <c r="B240" s="5">
+        <v>42596</v>
+      </c>
+      <c r="E240" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" s="4">
+        <f t="shared" si="10"/>
+        <v>42597</v>
+      </c>
+      <c r="B241" s="5">
+        <v>42597</v>
+      </c>
+      <c r="E241" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A242" s="4">
+        <f t="shared" si="10"/>
+        <v>42598</v>
+      </c>
+      <c r="B242" s="5">
+        <v>42598</v>
+      </c>
+      <c r="E242" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A243" s="4">
+        <f t="shared" si="10"/>
+        <v>42599</v>
+      </c>
+      <c r="B243" s="5">
+        <v>42599</v>
+      </c>
+      <c r="E243" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A244" s="4">
+        <f t="shared" si="10"/>
+        <v>42600</v>
+      </c>
+      <c r="B244" s="5">
+        <v>42600</v>
+      </c>
+      <c r="E244" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A245" s="4">
+        <f t="shared" si="10"/>
+        <v>42601</v>
+      </c>
+      <c r="B245" s="5">
+        <v>42601</v>
+      </c>
+      <c r="E245" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A246" s="4">
+        <f t="shared" si="10"/>
+        <v>42602</v>
+      </c>
+      <c r="B246" s="5">
+        <v>42602</v>
+      </c>
+      <c r="E246" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A247" s="4">
+        <f t="shared" si="10"/>
+        <v>42603</v>
+      </c>
+      <c r="B247" s="5">
+        <v>42603</v>
+      </c>
+      <c r="E247" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A248" s="4">
+        <f t="shared" si="10"/>
+        <v>42604</v>
+      </c>
+      <c r="B248" s="5">
+        <v>42604</v>
+      </c>
+      <c r="E248" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A249" s="4">
+        <f t="shared" si="10"/>
+        <v>42605</v>
+      </c>
+      <c r="B249" s="5">
+        <v>42605</v>
+      </c>
+      <c r="E249" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A250" s="4">
+        <f t="shared" si="10"/>
+        <v>42606</v>
+      </c>
+      <c r="B250" s="5">
+        <v>42606</v>
+      </c>
+      <c r="E250" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A251" s="4">
+        <f t="shared" si="10"/>
+        <v>42607</v>
+      </c>
+      <c r="B251" s="5">
+        <v>42607</v>
+      </c>
+      <c r="E251" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A252" s="4">
+        <f t="shared" si="10"/>
+        <v>42608</v>
+      </c>
+      <c r="B252" s="5">
+        <v>42608</v>
+      </c>
+      <c r="E252" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A253" s="4">
+        <f t="shared" si="10"/>
+        <v>42609</v>
+      </c>
+      <c r="B253" s="5">
+        <v>42609</v>
+      </c>
+      <c r="E253" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A254" s="4">
+        <f t="shared" si="10"/>
+        <v>42610</v>
+      </c>
+      <c r="B254" s="5">
+        <v>42610</v>
+      </c>
+      <c r="E254" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A255" s="4">
+        <f t="shared" si="10"/>
+        <v>42611</v>
+      </c>
+      <c r="B255" s="5">
+        <v>42611</v>
+      </c>
+      <c r="E255" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A256" s="4">
+        <f t="shared" si="10"/>
+        <v>42612</v>
+      </c>
+      <c r="B256" s="5">
+        <v>42612</v>
+      </c>
+      <c r="E256" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A257" s="4">
+        <f t="shared" si="10"/>
+        <v>42613</v>
+      </c>
+      <c r="B257" s="5">
+        <v>42613</v>
+      </c>
+      <c r="E257" s="2">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A258" s="4">
+        <f t="shared" si="10"/>
+        <v>42614</v>
+      </c>
+      <c r="B258" s="5">
+        <v>42614</v>
+      </c>
+      <c r="E258" s="2">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>